<commit_message>
Atualiza Tabela de Vendas - 06/05/2025
</commit_message>
<xml_diff>
--- a/Tabela de Vendas.xlsx
+++ b/Tabela de Vendas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93a171cd05344aea/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F8CFDE0-C913-48A1-8DD8-97494B17843F}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48C321EC-8B98-4F2E-9702-6EEE94968931}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="240" windowWidth="20730" windowHeight="11400" xr2:uid="{59A1ECAF-35FB-47A3-89C9-E4F516ECA120}"/>
+    <workbookView xWindow="-240" yWindow="360" windowWidth="20730" windowHeight="11400" xr2:uid="{59A1ECAF-35FB-47A3-89C9-E4F516ECA120}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" r:id="rId1"/>
@@ -381,58 +381,58 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -444,33 +444,6 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -651,6 +624,33 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -677,29 +677,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}" name="Tabela1" displayName="Tabela1" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}" name="Tabela1" displayName="Tabela1" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:T1048576" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{F4407804-865A-4282-AE09-A6A9CC885F74}" name="Data" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{C2A611FD-BE7A-4E94-B771-07A9FFEB611F}" name="Loja" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{D1C38DF9-9A9F-4D51-9460-F97844D4D328}" name="Referencia" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C2534D39-44D9-4D73-9D92-0D49C7FFFFAA}" name="Nº" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{C1D5464C-2768-4FF6-B1D8-BE54C1E70F16}" name="Marca" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{073D2F1E-E2E4-42F3-8617-1B0E9DA7018D}" name="Modelo" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{C5052134-A077-455A-B819-7C25015C936B}" name="Valor do Custo" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{53661555-6A99-4FCE-849F-4EE1140FEDF8}" name="Valor de Venda" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{67D3F8F8-8080-4C16-B69E-AFE60865BF82}" name="Qtde" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{A42F38F0-F689-4560-9395-84FFC37CDE13}" name="Valor  Vendido" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{721A3595-0194-44E0-A747-40C949AFC786}" name="Total Vendas" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{99D45803-3951-43FF-B2F7-0339881E78F6}" name="Desc %" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{67FBD3E1-E16C-4EF5-ABE6-8BECF71A094F}" name="Valor Desconto" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{FF20C066-1E57-41F5-964F-649BF22CDA8D}" name="Pagar Sapato" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{813D2FFE-B957-4B1F-B1E1-377A301E6C1E}" name="Custos do dia" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{1A4887F9-D3B7-42F2-833B-91209D9152AF}" name="Alimentação" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{AAFD2864-F209-4C7A-B3A6-069F0D7FE657}" name="Margem" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{B70D036C-9794-48E7-ACED-18B6E6097EB4}" name="Lucro total" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{3C99D4B6-3E27-41D5-9D82-466CCE3248A7}" name="R$ 2,00" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{C434B372-79FD-47AF-97E1-687634B5DF6D}" name="Acerto" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F4407804-865A-4282-AE09-A6A9CC885F74}" name="Data" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{C2A611FD-BE7A-4E94-B771-07A9FFEB611F}" name="Loja" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{D1C38DF9-9A9F-4D51-9460-F97844D4D328}" name="Referencia" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{C2534D39-44D9-4D73-9D92-0D49C7FFFFAA}" name="Nº" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{C1D5464C-2768-4FF6-B1D8-BE54C1E70F16}" name="Marca" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{073D2F1E-E2E4-42F3-8617-1B0E9DA7018D}" name="Modelo" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{C5052134-A077-455A-B819-7C25015C936B}" name="Valor do Custo" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{53661555-6A99-4FCE-849F-4EE1140FEDF8}" name="Valor de Venda" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{67D3F8F8-8080-4C16-B69E-AFE60865BF82}" name="Qtde" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{A42F38F0-F689-4560-9395-84FFC37CDE13}" name="Valor  Vendido" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{721A3595-0194-44E0-A747-40C949AFC786}" name="Total Vendas" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{99D45803-3951-43FF-B2F7-0339881E78F6}" name="Desc %" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{67FBD3E1-E16C-4EF5-ABE6-8BECF71A094F}" name="Valor Desconto" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{FF20C066-1E57-41F5-964F-649BF22CDA8D}" name="Pagar Sapato" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{813D2FFE-B957-4B1F-B1E1-377A301E6C1E}" name="Custos do dia" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{1A4887F9-D3B7-42F2-833B-91209D9152AF}" name="Alimentação" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{AAFD2864-F209-4C7A-B3A6-069F0D7FE657}" name="Margem" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{B70D036C-9794-48E7-ACED-18B6E6097EB4}" name="Lucro total" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{3C99D4B6-3E27-41D5-9D82-466CCE3248A7}" name="R$ 2,00" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{C434B372-79FD-47AF-97E1-687634B5DF6D}" name="Acerto" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1024,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9C7257-E4EF-46C5-A436-4891D3BFE8E4}">
   <dimension ref="A1:Y306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A284" sqref="A284"/>
+    <sheetView tabSelected="1" topLeftCell="K283" workbookViewId="0">
+      <selection activeCell="U304" sqref="U304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17161,7 +17161,7 @@
       <c r="S283" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="U283" s="10">
+      <c r="U283" s="14">
         <f>S304</f>
         <v>55</v>
       </c>
@@ -18136,7 +18136,7 @@
         <f>R304/S282</f>
         <v>55</v>
       </c>
-      <c r="U304" s="10">
+      <c r="U304" s="14">
         <f>U283-W304</f>
         <v>-440.32000000000005</v>
       </c>

</xml_diff>

<commit_message>
Atualiza Tabela de Vendas - 07/05/2025
</commit_message>
<xml_diff>
--- a/Tabela de Vendas.xlsx
+++ b/Tabela de Vendas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93a171cd05344aea/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B35BB166-1E22-47DF-8DAC-C9DB35CAAEE1}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A25292F4-8E5C-4748-97D8-543C71ABBED6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="240" windowWidth="20730" windowHeight="11400" xr2:uid="{59A1ECAF-35FB-47A3-89C9-E4F516ECA120}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="84">
   <si>
     <t>Data</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>condominio</t>
-  </si>
-  <si>
-    <t>teste</t>
   </si>
 </sst>
 </file>
@@ -1027,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9C7257-E4EF-46C5-A436-4891D3BFE8E4}">
   <dimension ref="A1:Y306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K283" workbookViewId="0">
-      <selection activeCell="X291" sqref="X291"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="X302" sqref="X302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17159,14 +17156,14 @@
       </c>
       <c r="R283" s="14">
         <f>SUM(R284:R302)</f>
-        <v>160</v>
+        <v>452</v>
       </c>
       <c r="S283" s="14" t="s">
         <v>27</v>
       </c>
       <c r="U283" s="14">
         <f>S304</f>
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="W283" s="16">
         <v>135</v>
@@ -17292,7 +17289,9 @@
         <f t="shared" si="83"/>
         <v>100</v>
       </c>
-      <c r="O285" s="10"/>
+      <c r="O285" s="10">
+        <v>20</v>
+      </c>
       <c r="P285" s="10"/>
       <c r="Q285" s="12">
         <f t="shared" si="84"/>
@@ -17314,45 +17313,65 @@
       </c>
     </row>
     <row r="286" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="1"/>
-      <c r="B286" s="5"/>
-      <c r="C286" s="3"/>
-      <c r="D286" s="3"/>
-      <c r="E286" s="3"/>
-      <c r="F286" s="5"/>
-      <c r="G286" s="10"/>
-      <c r="H286" s="10"/>
-      <c r="I286" s="3"/>
-      <c r="J286" s="10"/>
+      <c r="A286" s="1">
+        <v>45784</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C286" s="3">
+        <v>2188</v>
+      </c>
+      <c r="D286" s="3">
+        <v>38</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F286" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G286" s="10">
+        <v>100</v>
+      </c>
+      <c r="H286" s="10">
+        <v>199</v>
+      </c>
+      <c r="I286" s="3">
+        <v>1</v>
+      </c>
+      <c r="J286" s="10">
+        <v>180</v>
+      </c>
       <c r="K286" s="10">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L286" s="12" t="str">
+        <v>180</v>
+      </c>
+      <c r="L286" s="12">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M286" s="10" t="str">
+        <v>9.5477386934673336E-2</v>
+      </c>
+      <c r="M286" s="10">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>18.999999999999993</v>
       </c>
       <c r="N286" s="10">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O286" s="10"/>
       <c r="P286" s="10"/>
-      <c r="Q286" s="12" t="str">
+      <c r="Q286" s="12">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="R286" s="10">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="S286" s="10">
         <f>R286/S282</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W286" s="16">
         <v>33.33</v>
@@ -17362,45 +17381,65 @@
       </c>
     </row>
     <row r="287" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
-      <c r="B287" s="5"/>
-      <c r="C287" s="3"/>
-      <c r="D287" s="3"/>
-      <c r="E287" s="3"/>
-      <c r="F287" s="5"/>
-      <c r="G287" s="10"/>
-      <c r="H287" s="10"/>
-      <c r="I287" s="3"/>
-      <c r="J287" s="10"/>
+      <c r="A287" s="1">
+        <v>45784</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C287" s="3">
+        <v>1046</v>
+      </c>
+      <c r="D287" s="3">
+        <v>39</v>
+      </c>
+      <c r="E287" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F287" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G287" s="10">
+        <v>50</v>
+      </c>
+      <c r="H287" s="10">
+        <v>110</v>
+      </c>
+      <c r="I287" s="3">
+        <v>1</v>
+      </c>
+      <c r="J287" s="10">
+        <v>100</v>
+      </c>
       <c r="K287" s="10">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L287" s="12" t="str">
+        <v>100</v>
+      </c>
+      <c r="L287" s="12">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M287" s="10" t="str">
+        <v>9.0909090909090939E-2</v>
+      </c>
+      <c r="M287" s="10">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>10.000000000000004</v>
       </c>
       <c r="N287" s="10">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O287" s="10"/>
       <c r="P287" s="10"/>
-      <c r="Q287" s="12" t="str">
+      <c r="Q287" s="12">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.5</v>
       </c>
       <c r="R287" s="10">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S287" s="10">
         <f>R287/S282</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="W287" s="16">
         <v>81.900000000000006</v>
@@ -17410,45 +17449,65 @@
       </c>
     </row>
     <row r="288" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="1"/>
-      <c r="B288" s="5"/>
-      <c r="C288" s="3"/>
-      <c r="D288" s="3"/>
-      <c r="E288" s="3"/>
-      <c r="F288" s="5"/>
-      <c r="G288" s="10"/>
-      <c r="H288" s="10"/>
-      <c r="I288" s="3"/>
-      <c r="J288" s="10"/>
+      <c r="A288" s="1">
+        <v>45784</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C288" s="3">
+        <v>5500</v>
+      </c>
+      <c r="D288" s="3">
+        <v>39</v>
+      </c>
+      <c r="E288" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F288" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G288" s="10">
+        <v>112</v>
+      </c>
+      <c r="H288" s="10">
+        <v>190</v>
+      </c>
+      <c r="I288" s="3">
+        <v>1</v>
+      </c>
+      <c r="J288" s="10">
+        <v>190</v>
+      </c>
       <c r="K288" s="10">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L288" s="12" t="str">
+        <v>190</v>
+      </c>
+      <c r="L288" s="12">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M288" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="M288" s="10">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="N288" s="10">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O288" s="10"/>
       <c r="P288" s="10"/>
-      <c r="Q288" s="12" t="str">
+      <c r="Q288" s="12">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.41052631578947368</v>
       </c>
       <c r="R288" s="10">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="S288" s="10">
         <f>R288/S282</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="W288" s="16">
         <v>18</v>
@@ -17458,45 +17517,65 @@
       </c>
     </row>
     <row r="289" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="1"/>
-      <c r="B289" s="5"/>
-      <c r="C289" s="3"/>
-      <c r="D289" s="3"/>
-      <c r="E289" s="3"/>
-      <c r="F289" s="5"/>
-      <c r="G289" s="10"/>
-      <c r="H289" s="10"/>
-      <c r="I289" s="3"/>
-      <c r="J289" s="10"/>
+      <c r="A289" s="1">
+        <v>45784</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C289" s="3">
+        <v>400</v>
+      </c>
+      <c r="D289" s="3">
+        <v>40</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F289" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G289" s="10">
+        <v>126</v>
+      </c>
+      <c r="H289" s="10">
+        <v>210</v>
+      </c>
+      <c r="I289" s="3">
+        <v>1</v>
+      </c>
+      <c r="J289" s="10">
+        <v>210</v>
+      </c>
       <c r="K289" s="10">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L289" s="12" t="str">
+        <v>210</v>
+      </c>
+      <c r="L289" s="12">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M289" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="M289" s="10">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="N289" s="10">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="O289" s="10"/>
       <c r="P289" s="10"/>
-      <c r="Q289" s="12" t="str">
+      <c r="Q289" s="12">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.4</v>
       </c>
       <c r="R289" s="10">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="S289" s="10">
         <f>R289/S282</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="W289" s="16">
         <v>35</v>
@@ -17593,12 +17672,6 @@
         <f>R291/S282</f>
         <v>0</v>
       </c>
-      <c r="W291" s="4">
-        <v>10</v>
-      </c>
-      <c r="X291" s="4" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="292" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
@@ -18109,25 +18182,25 @@
       <c r="H304" s="10"/>
       <c r="I304" s="13">
         <f xml:space="preserve"> SUM(I284:I303)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J304" s="10"/>
       <c r="K304" s="14">
         <f>SUM(K284:K303)</f>
-        <v>360</v>
+        <v>1040</v>
       </c>
       <c r="L304" s="15"/>
       <c r="M304" s="14">
         <f>SUM(M284:M303)</f>
-        <v>37.999999999999986</v>
+        <v>66.999999999999986</v>
       </c>
       <c r="N304" s="14">
         <f>SUM(N284:N303)</f>
-        <v>200</v>
+        <v>588</v>
       </c>
       <c r="O304" s="14">
         <f>SUM(O284:O303)</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="P304" s="14">
         <f>SUM(P284:P303)</f>
@@ -18135,23 +18208,23 @@
       </c>
       <c r="Q304" s="15">
         <f>IF(R304,R304/K304,0)</f>
-        <v>0.30555555555555558</v>
+        <v>0.36730769230769234</v>
       </c>
       <c r="R304" s="14">
         <f>R283-O304-P304</f>
-        <v>110</v>
+        <v>382</v>
       </c>
       <c r="S304" s="14">
         <f>R304/S282</f>
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="U304" s="14">
         <f>U283-W304</f>
-        <v>-450.32000000000005</v>
-      </c>
-      <c r="W304" s="13">
+        <v>-304.32000000000005</v>
+      </c>
+      <c r="W304" s="17">
         <f>SUM(W283:W303)</f>
-        <v>505.32000000000005</v>
+        <v>495.32000000000005</v>
       </c>
     </row>
     <row r="305" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualiza Tabela de Vendas - 09/05/2025
</commit_message>
<xml_diff>
--- a/Tabela de Vendas.xlsx
+++ b/Tabela de Vendas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93a171cd05344aea/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36212238-9029-454B-97B1-61508BEE1EDD}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{099EF8D1-F0B8-4A21-9C18-DBFAC8BEA08E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="240" windowWidth="20730" windowHeight="11400" xr2:uid="{59A1ECAF-35FB-47A3-89C9-E4F516ECA120}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="85">
   <si>
     <t>Data</t>
   </si>
@@ -289,6 +289,9 @@
   <si>
     <t>condominio</t>
   </si>
+  <si>
+    <t xml:space="preserve">Laninha </t>
+  </si>
 </sst>
 </file>
 
@@ -370,49 +373,49 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -604,6 +607,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -645,16 +658,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -668,8 +671,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}" name="Tabela1" displayName="Tabela1" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}" name="Tabela1" displayName="Tabela1" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:T1048576" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{F4407804-865A-4282-AE09-A6A9CC885F74}" name="Data" dataDxfId="19"/>
@@ -1016,17 +1023,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9C7257-E4EF-46C5-A436-4891D3BFE8E4}">
   <dimension ref="A1:Y306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="J290" sqref="J290"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="W295" sqref="W295"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="15" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="15" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="15" customWidth="1"/>
@@ -14404,7 +14411,7 @@
       <c r="S235" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="U235" s="9">
+      <c r="U235" s="11">
         <f>S256+S280</f>
         <v>864.15000000000009</v>
       </c>
@@ -17148,14 +17155,14 @@
       </c>
       <c r="R283" s="11">
         <f>SUM(R284:R302)</f>
-        <v>541</v>
+        <v>703</v>
       </c>
       <c r="S283" s="11" t="s">
         <v>27</v>
       </c>
       <c r="U283" s="11">
         <f>S304</f>
-        <v>235.5</v>
+        <v>316.5</v>
       </c>
       <c r="W283" s="13">
         <v>135</v>
@@ -17645,86 +17652,133 @@
       </c>
     </row>
     <row r="291" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="1"/>
-      <c r="B291" s="6"/>
-      <c r="C291" s="6"/>
-      <c r="D291" s="6"/>
-      <c r="F291" s="4"/>
-      <c r="G291" s="3"/>
-      <c r="H291" s="3"/>
-      <c r="I291" s="6"/>
-      <c r="J291" s="3"/>
+      <c r="A291" s="1">
+        <v>45786</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C291" s="6">
+        <v>2085</v>
+      </c>
+      <c r="D291" s="6">
+        <v>41</v>
+      </c>
+      <c r="E291" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F291" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G291" s="3">
+        <v>100</v>
+      </c>
+      <c r="H291" s="3">
+        <v>199</v>
+      </c>
+      <c r="I291" s="6">
+        <v>1</v>
+      </c>
+      <c r="J291" s="3">
+        <v>175</v>
+      </c>
       <c r="K291" s="3">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L291" s="4" t="str">
+        <v>175</v>
+      </c>
+      <c r="L291" s="4">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M291" s="3" t="str">
+        <v>0.12060301507537685</v>
+      </c>
+      <c r="M291" s="3">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>23.999999999999993</v>
       </c>
       <c r="N291" s="3">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O291" s="3"/>
       <c r="P291" s="3"/>
-      <c r="Q291" s="4" t="str">
+      <c r="Q291" s="4">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="R291" s="3">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="S291" s="3">
         <f>R291/S282</f>
-        <v>0</v>
+        <v>37.5</v>
+      </c>
+      <c r="W291" s="13">
+        <v>75</v>
+      </c>
+      <c r="X291" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="292" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="1"/>
-      <c r="B292" s="6"/>
-      <c r="C292" s="6"/>
-      <c r="D292" s="6"/>
-      <c r="E292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="G292" s="3"/>
-      <c r="H292" s="3"/>
-      <c r="I292" s="6"/>
-      <c r="J292" s="3"/>
+      <c r="A292" s="1">
+        <v>45786</v>
+      </c>
+      <c r="B292" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C292" s="6">
+        <v>5500</v>
+      </c>
+      <c r="D292" s="6">
+        <v>40</v>
+      </c>
+      <c r="E292" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F292" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G292" s="3">
+        <v>112</v>
+      </c>
+      <c r="H292" s="3">
+        <v>190</v>
+      </c>
+      <c r="I292" s="6">
+        <v>1</v>
+      </c>
+      <c r="J292" s="3">
+        <v>199</v>
+      </c>
       <c r="K292" s="3">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L292" s="4" t="str">
+        <v>199</v>
+      </c>
+      <c r="L292" s="4">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M292" s="3" t="str">
+        <v>-4.7368421052631504E-2</v>
+      </c>
+      <c r="M292" s="3">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>-8.9999999999999858</v>
       </c>
       <c r="N292" s="3">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O292" s="3"/>
       <c r="P292" s="3"/>
-      <c r="Q292" s="4" t="str">
+      <c r="Q292" s="4">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.43718592964824121</v>
       </c>
       <c r="R292" s="3">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="S292" s="3">
         <f>R292/S282</f>
-        <v>0</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="293" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -18194,21 +18248,21 @@
       <c r="H304" s="3"/>
       <c r="I304" s="9">
         <f xml:space="preserve"> SUM(I284:I303)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J304" s="3"/>
       <c r="K304" s="11">
         <f>SUM(K284:K303)</f>
-        <v>1229</v>
+        <v>1603</v>
       </c>
       <c r="L304" s="12"/>
       <c r="M304" s="11">
         <f>SUM(M284:M303)</f>
-        <v>76.999999999999986</v>
+        <v>91.999999999999986</v>
       </c>
       <c r="N304" s="11">
         <f>SUM(N284:N303)</f>
-        <v>688</v>
+        <v>900</v>
       </c>
       <c r="O304" s="11">
         <f>SUM(O284:O303)</f>
@@ -18220,23 +18274,23 @@
       </c>
       <c r="Q304" s="12">
         <f>IF(R304,R304/K304,0)</f>
-        <v>0.38323840520748575</v>
+        <v>0.39488459139114163</v>
       </c>
       <c r="R304" s="11">
         <f>R283-O304-P304</f>
-        <v>471</v>
+        <v>633</v>
       </c>
       <c r="S304" s="11">
         <f>R304/S282</f>
-        <v>235.5</v>
+        <v>316.5</v>
       </c>
       <c r="U304" s="11">
         <f>U283-W304</f>
-        <v>-259.82000000000005</v>
+        <v>-253.82000000000005</v>
       </c>
       <c r="W304" s="14">
         <f>SUM(W283:W303)</f>
-        <v>495.32000000000005</v>
+        <v>570.32000000000005</v>
       </c>
     </row>
     <row r="305" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -18271,8 +18325,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualiza Tabela de Vendas - 11/05/2025
</commit_message>
<xml_diff>
--- a/Tabela de Vendas.xlsx
+++ b/Tabela de Vendas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93a171cd05344aea/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{AAFE6087-9843-4B6B-A287-947E675793D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{099EF8D1-F0B8-4A21-9C18-DBFAC8BEA08E}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1000001_{B4D4F34F-2D88-5B42-9D3D-5F73FFD5704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DDFE2DE-6AEC-4066-A549-59D0E830CD7A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="240" windowWidth="20730" windowHeight="11400" xr2:uid="{59A1ECAF-35FB-47A3-89C9-E4F516ECA120}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="86">
   <si>
     <t>Data</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t xml:space="preserve">Laninha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3x tênis </t>
   </si>
 </sst>
 </file>
@@ -671,10 +674,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}" name="Tabela1" displayName="Tabela1" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:T1048576" xr:uid="{0F7915E7-DFCA-4A1A-A535-0BC68CF2610C}"/>
@@ -1023,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9C7257-E4EF-46C5-A436-4891D3BFE8E4}">
   <dimension ref="A1:Y306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="W295" sqref="W295"/>
+    <sheetView tabSelected="1" topLeftCell="Q291" workbookViewId="0">
+      <selection activeCell="X306" sqref="X306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17155,14 +17154,14 @@
       </c>
       <c r="R283" s="11">
         <f>SUM(R284:R302)</f>
-        <v>703</v>
+        <v>934</v>
       </c>
       <c r="S283" s="11" t="s">
         <v>27</v>
       </c>
       <c r="U283" s="11">
         <f>S304</f>
-        <v>316.5</v>
+        <v>422</v>
       </c>
       <c r="W283" s="13">
         <v>135</v>
@@ -17358,7 +17357,9 @@
         <f t="shared" si="83"/>
         <v>100</v>
       </c>
-      <c r="O286" s="3"/>
+      <c r="O286" s="3">
+        <v>20</v>
+      </c>
       <c r="P286" s="3"/>
       <c r="Q286" s="4">
         <f t="shared" si="84"/>
@@ -17612,19 +17613,19 @@
         <v>1</v>
       </c>
       <c r="J290" s="3">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="K290" s="3">
         <f t="shared" si="80"/>
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="L290" s="4">
         <f t="shared" si="81"/>
-        <v>5.0251256281407031E-2</v>
+        <v>9.5477386934673336E-2</v>
       </c>
       <c r="M290" s="3">
         <f t="shared" si="82"/>
-        <v>10</v>
+        <v>18.999999999999993</v>
       </c>
       <c r="N290" s="3">
         <f t="shared" si="83"/>
@@ -17634,15 +17635,15 @@
       <c r="P290" s="3"/>
       <c r="Q290" s="4">
         <f t="shared" si="84"/>
-        <v>0.47089947089947087</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="R290" s="3">
         <f t="shared" si="85"/>
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="S290" s="3">
         <f>R290/S282</f>
-        <v>44.5</v>
+        <v>40</v>
       </c>
       <c r="W290" s="13">
         <v>121.99</v>
@@ -17782,171 +17783,251 @@
       </c>
     </row>
     <row r="293" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A293" s="1"/>
-      <c r="B293" s="6"/>
-      <c r="C293" s="6"/>
-      <c r="D293" s="6"/>
-      <c r="E293" s="6"/>
-      <c r="F293" s="6"/>
-      <c r="G293" s="3"/>
-      <c r="H293" s="3"/>
-      <c r="I293" s="6"/>
-      <c r="J293" s="3"/>
+      <c r="A293" s="1">
+        <v>45787</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C293" s="6">
+        <v>2188</v>
+      </c>
+      <c r="D293" s="6">
+        <v>39</v>
+      </c>
+      <c r="E293" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F293" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G293" s="3">
+        <v>100</v>
+      </c>
+      <c r="H293" s="3">
+        <v>199</v>
+      </c>
+      <c r="I293" s="6">
+        <v>1</v>
+      </c>
+      <c r="J293" s="3">
+        <v>190</v>
+      </c>
       <c r="K293" s="3">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L293" s="4" t="str">
+        <v>190</v>
+      </c>
+      <c r="L293" s="4">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M293" s="3" t="str">
+        <v>4.5226130653266305E-2</v>
+      </c>
+      <c r="M293" s="3">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>8.9999999999999947</v>
       </c>
       <c r="N293" s="3">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O293" s="3"/>
       <c r="P293" s="3"/>
-      <c r="Q293" s="4" t="str">
+      <c r="Q293" s="4">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.47368421052631576</v>
       </c>
       <c r="R293" s="3">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="S293" s="3">
         <f>R293/S282</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="294" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="1"/>
-      <c r="B294" s="6"/>
-      <c r="C294" s="6"/>
-      <c r="D294" s="6"/>
-      <c r="E294" s="6"/>
-      <c r="F294" s="6"/>
-      <c r="G294" s="3"/>
-      <c r="H294" s="3"/>
-      <c r="I294" s="6"/>
-      <c r="J294" s="3"/>
+      <c r="A294" s="1">
+        <v>45787</v>
+      </c>
+      <c r="B294" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C294" s="6">
+        <v>1046</v>
+      </c>
+      <c r="D294" s="6">
+        <v>39</v>
+      </c>
+      <c r="E294" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F294" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G294" s="3">
+        <v>50</v>
+      </c>
+      <c r="H294" s="3">
+        <v>110</v>
+      </c>
+      <c r="I294" s="6">
+        <v>1</v>
+      </c>
+      <c r="J294" s="3">
+        <v>100</v>
+      </c>
       <c r="K294" s="3">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L294" s="4" t="str">
+        <v>100</v>
+      </c>
+      <c r="L294" s="4">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M294" s="3" t="str">
+        <v>9.0909090909090939E-2</v>
+      </c>
+      <c r="M294" s="3">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>10.000000000000004</v>
       </c>
       <c r="N294" s="3">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O294" s="3"/>
       <c r="P294" s="3"/>
-      <c r="Q294" s="4" t="str">
+      <c r="Q294" s="4">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.5</v>
       </c>
       <c r="R294" s="3">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S294" s="3">
         <f>R294/S282</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="295" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="1"/>
-      <c r="B295" s="6"/>
-      <c r="C295" s="6"/>
-      <c r="D295" s="6"/>
-      <c r="E295" s="6"/>
-      <c r="F295" s="6"/>
-      <c r="G295" s="3"/>
-      <c r="H295" s="3"/>
-      <c r="I295" s="6"/>
-      <c r="J295" s="3"/>
+      <c r="A295" s="1">
+        <v>45787</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C295" s="6">
+        <v>1046</v>
+      </c>
+      <c r="D295" s="6">
+        <v>40</v>
+      </c>
+      <c r="E295" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F295" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G295" s="3">
+        <v>50</v>
+      </c>
+      <c r="H295" s="3">
+        <v>110</v>
+      </c>
+      <c r="I295" s="6">
+        <v>1</v>
+      </c>
+      <c r="J295" s="3">
+        <v>100</v>
+      </c>
       <c r="K295" s="3">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L295" s="4" t="str">
+        <v>100</v>
+      </c>
+      <c r="L295" s="4">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M295" s="3" t="str">
+        <v>9.0909090909090939E-2</v>
+      </c>
+      <c r="M295" s="3">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>10.000000000000004</v>
       </c>
       <c r="N295" s="3">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O295" s="3"/>
       <c r="P295" s="3"/>
-      <c r="Q295" s="4" t="str">
+      <c r="Q295" s="4">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.5</v>
       </c>
       <c r="R295" s="3">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S295" s="3">
         <f>R295/S282</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="296" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="1"/>
-      <c r="B296" s="6"/>
-      <c r="C296" s="6"/>
-      <c r="D296" s="6"/>
-      <c r="E296" s="6"/>
-      <c r="F296" s="6"/>
-      <c r="G296" s="3"/>
-      <c r="H296" s="3"/>
-      <c r="I296" s="6"/>
-      <c r="J296" s="3"/>
+      <c r="A296" s="1">
+        <v>45787</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C296" s="6">
+        <v>1046</v>
+      </c>
+      <c r="D296" s="6">
+        <v>43</v>
+      </c>
+      <c r="E296" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F296" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G296" s="3">
+        <v>50</v>
+      </c>
+      <c r="H296" s="3">
+        <v>110</v>
+      </c>
+      <c r="I296" s="6">
+        <v>1</v>
+      </c>
+      <c r="J296" s="3">
+        <v>100</v>
+      </c>
       <c r="K296" s="3">
         <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="L296" s="4" t="str">
+        <v>100</v>
+      </c>
+      <c r="L296" s="4">
         <f t="shared" si="81"/>
-        <v>-</v>
-      </c>
-      <c r="M296" s="3" t="str">
+        <v>9.0909090909090939E-2</v>
+      </c>
+      <c r="M296" s="3">
         <f t="shared" si="82"/>
-        <v>-</v>
+        <v>10.000000000000004</v>
       </c>
       <c r="N296" s="3">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O296" s="3"/>
       <c r="P296" s="3"/>
-      <c r="Q296" s="4" t="str">
+      <c r="Q296" s="4">
         <f t="shared" si="84"/>
-        <v>-</v>
+        <v>0.5</v>
       </c>
       <c r="R296" s="3">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S296" s="3">
         <f>R296/S282</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="297" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -18248,25 +18329,25 @@
       <c r="H304" s="3"/>
       <c r="I304" s="9">
         <f xml:space="preserve"> SUM(I284:I303)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J304" s="3"/>
       <c r="K304" s="11">
         <f>SUM(K284:K303)</f>
-        <v>1603</v>
+        <v>2084</v>
       </c>
       <c r="L304" s="12"/>
       <c r="M304" s="11">
         <f>SUM(M284:M303)</f>
-        <v>91.999999999999986</v>
+        <v>140</v>
       </c>
       <c r="N304" s="11">
         <f>SUM(N284:N303)</f>
-        <v>900</v>
+        <v>1150</v>
       </c>
       <c r="O304" s="11">
         <f>SUM(O284:O303)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="P304" s="11">
         <f>SUM(P284:P303)</f>
@@ -18274,26 +18355,26 @@
       </c>
       <c r="Q304" s="12">
         <f>IF(R304,R304/K304,0)</f>
-        <v>0.39488459139114163</v>
+        <v>0.4049904030710173</v>
       </c>
       <c r="R304" s="11">
         <f>R283-O304-P304</f>
-        <v>633</v>
+        <v>844</v>
       </c>
       <c r="S304" s="11">
         <f>R304/S282</f>
-        <v>316.5</v>
+        <v>422</v>
       </c>
       <c r="U304" s="11">
         <f>U283-W304</f>
-        <v>-253.82000000000005</v>
+        <v>-148.32000000000005</v>
       </c>
       <c r="W304" s="14">
         <f>SUM(W283:W303)</f>
         <v>570.32000000000005</v>
       </c>
     </row>
-    <row r="305" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="G305" s="3"/>
       <c r="H305" s="3"/>
@@ -18308,7 +18389,7 @@
       <c r="R305" s="3"/>
       <c r="S305" s="3"/>
     </row>
-    <row r="306" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1"/>
       <c r="G306" s="3"/>
       <c r="H306" s="3"/>
@@ -18322,6 +18403,12 @@
       <c r="Q306" s="4"/>
       <c r="R306" s="3"/>
       <c r="S306" s="3"/>
+      <c r="W306" s="2">
+        <v>160</v>
+      </c>
+      <c r="X306" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>